<commit_message>
feat: :sparkles: new coding for rhythm and music not synch
also reduce animation time for slot machine
</commit_message>
<xml_diff>
--- a/LEGENDA_CODIFICA.xlsx
+++ b/LEGENDA_CODIFICA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ilaria\Documenti\POLIMI\corsi\AUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLI_sw\Unity\projects\C(H)o(L)ordination\C(H)o(L)ordination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9039A6B3-CE93-4466-AB3D-2D31A2AC6F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691BF63D-D1E8-4E1A-9728-7631AD107F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2239" yWindow="419" windowWidth="20225" windowHeight="12292" xr2:uid="{EDEB0BF4-CBE7-4800-BCC3-C1EC8D52E7B3}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{EDEB0BF4-CBE7-4800-BCC3-C1EC8D52E7B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
-  <si>
-    <t>TIPO ATTIVITA'</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>COSTANTE</t>
   </si>
@@ -113,6 +110,15 @@
   </si>
   <si>
     <t xml:space="preserve">Se il timer è diverso da "-1" allora è il tempo che il pianeta impiega per passare attraverso la zona gialla oppure quanto il soggetto impiega ad interagirci </t>
+  </si>
+  <si>
+    <t>MUSICA ATTIVA</t>
+  </si>
+  <si>
+    <t>RITMO ATTIVO</t>
+  </si>
+  <si>
+    <t>NESSUN SUONO</t>
   </si>
 </sst>
 </file>
@@ -621,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5334469-10E7-419C-ACB8-CF35FB7AA93B}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -630,81 +636,113 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="13" t="s">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
         <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="C5" s="3">
+        <v>110</v>
+      </c>
+      <c r="D5" s="3">
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>2</v>
+        <v>200</v>
+      </c>
+      <c r="C6" s="3">
+        <v>210</v>
+      </c>
+      <c r="D6" s="3">
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4">
-        <v>3</v>
+        <v>300</v>
+      </c>
+      <c r="C7" s="4">
+        <v>310</v>
+      </c>
+      <c r="D7" s="4">
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="7">
         <v>11</v>
@@ -714,28 +752,28 @@
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
         <v>10</v>
@@ -743,7 +781,7 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4">
         <v>11</v>
@@ -752,7 +790,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
@@ -766,18 +804,18 @@
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>18</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="2">
         <v>100</v>
@@ -785,10 +823,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="3">
         <v>101</v>
@@ -796,10 +834,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="3">
         <v>110</v>
@@ -807,10 +845,10 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="4">
         <v>111</v>
@@ -818,7 +856,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: :bug: bug in the encoding of scene difficulty after last changes
also renaming for consistency
</commit_message>
<xml_diff>
--- a/LEGENDA_CODIFICA.xlsx
+++ b/LEGENDA_CODIFICA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLI_sw\Unity\projects\C(H)o(L)ordination\C(H)o(L)ordination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691BF63D-D1E8-4E1A-9728-7631AD107F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6720D0FC-4E0F-4F82-8B81-A9448B5BCF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{EDEB0BF4-CBE7-4800-BCC3-C1EC8D52E7B3}"/>
+    <workbookView xWindow="5079" yWindow="1375" windowWidth="17490" windowHeight="12855" tabRatio="319" xr2:uid="{EDEB0BF4-CBE7-4800-BCC3-C1EC8D52E7B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>COSTANTE</t>
   </si>
@@ -112,23 +112,54 @@
     <t xml:space="preserve">Se il timer è diverso da "-1" allora è il tempo che il pianeta impiega per passare attraverso la zona gialla oppure quanto il soggetto impiega ad interagirci </t>
   </si>
   <si>
-    <t>MUSICA ATTIVA</t>
-  </si>
-  <si>
-    <t>RITMO ATTIVO</t>
-  </si>
-  <si>
     <t>NESSUN SUONO</t>
+  </si>
+  <si>
+    <t>_00000</t>
+  </si>
+  <si>
+    <t>_01000</t>
+  </si>
+  <si>
+    <t>_00100</t>
+  </si>
+  <si>
+    <t>_00010</t>
+  </si>
+  <si>
+    <t>_00001</t>
+  </si>
+  <si>
+    <t>RITMO ASYNCH</t>
+  </si>
+  <si>
+    <t>MUSICA ASYNCH</t>
+  </si>
+  <si>
+    <t>RITMO SYNCH</t>
+  </si>
+  <si>
+    <t>MUSICA SYNCH</t>
+  </si>
+  <si>
+    <t>il primo bit è il tipo dell'attività, quelli successivi sono 1 se attiva / 0 se non attiva la funzionalità corrispondente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -258,11 +289,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -274,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -283,7 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -308,8 +353,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -625,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5334469-10E7-419C-ACB8-CF35FB7AA93B}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -636,93 +683,146 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="C5" s="3">
-        <v>110</v>
+        <v>11000</v>
       </c>
       <c r="D5" s="3">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+        <v>10100</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10010</v>
+      </c>
+      <c r="F5" s="3">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>200</v>
+        <v>20000</v>
       </c>
       <c r="C6" s="3">
-        <v>210</v>
+        <v>21000</v>
       </c>
       <c r="D6" s="3">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+        <v>20100</v>
+      </c>
+      <c r="E6" s="3">
+        <v>20010</v>
+      </c>
+      <c r="F6" s="3">
+        <v>20001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4">
-        <v>300</v>
+        <v>30000</v>
       </c>
       <c r="C7" s="4">
-        <v>310</v>
+        <v>31000</v>
       </c>
       <c r="D7" s="4">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+        <v>30100</v>
+      </c>
+      <c r="E7" s="4">
+        <v>30010</v>
+      </c>
+      <c r="F7" s="4">
+        <v>30001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -731,135 +831,136 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:17" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="13" t="s">
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8"/>
+      <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="4">
         <v>11</v>
       </c>
-      <c r="M20" s="25"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="3">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="3">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="20" t="s">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="4">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="23" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H3:Q4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: :sparkles: adding harmonical movement constant speed scene
</commit_message>
<xml_diff>
--- a/LEGENDA_CODIFICA.xlsx
+++ b/LEGENDA_CODIFICA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLI_sw\Unity\projects\C(H)o(L)ordination\C(H)o(L)ordination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6720D0FC-4E0F-4F82-8B81-A9448B5BCF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DD33A7-C70B-4C2E-8F23-72174394F405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5079" yWindow="1375" windowWidth="17490" windowHeight="12855" tabRatio="319" xr2:uid="{EDEB0BF4-CBE7-4800-BCC3-C1EC8D52E7B3}"/>
+    <workbookView xWindow="1479" yWindow="668" windowWidth="22333" windowHeight="12855" tabRatio="319" xr2:uid="{EDEB0BF4-CBE7-4800-BCC3-C1EC8D52E7B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>COSTANTE</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>il primo bit è il tipo dell'attività, quelli successivi sono 1 se attiva / 0 se non attiva la funzionalità corrispondente</t>
+  </si>
+  <si>
+    <t>MOV. ARMONICO CONSTANTE</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -354,13 +357,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -376,7 +378,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -672,15 +674,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5334469-10E7-419C-ACB8-CF35FB7AA93B}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" customWidth="1"/>
@@ -814,146 +816,165 @@
         <v>30001</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="12" t="s">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4">
+        <v>40000</v>
+      </c>
+      <c r="C8" s="4">
+        <v>41000</v>
+      </c>
+      <c r="D8" s="4">
+        <v>40100</v>
+      </c>
+      <c r="E8" s="4">
+        <v>40010</v>
+      </c>
+      <c r="F8" s="4">
+        <v>40001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="24"/>
-    </row>
-    <row r="12" spans="1:17" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+    </row>
+    <row r="13" spans="1:17" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B14" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
-      <c r="B16" s="12" t="s">
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8"/>
+      <c r="B17" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B21" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="20" t="s">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C25" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C26" s="2">
         <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="3">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B28" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C28" s="3">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C29" s="4">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>